<commit_message>
update main.py to provinces level
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>市</t>
   </si>
@@ -110,6 +110,39 @@
   </si>
   <si>
     <t>https://www.xinji.gov.cn/html/czyjs_zfjs/index.html</t>
+  </si>
+  <si>
+    <t>保定市</t>
+  </si>
+  <si>
+    <t>涞水县</t>
+  </si>
+  <si>
+    <t>https://www.laishui.gov.cn/index.php?m=content&amp;c=index&amp;a=lists&amp;catid=173</t>
+  </si>
+  <si>
+    <t>阜平县</t>
+  </si>
+  <si>
+    <t>https://www.bdfuping.gov.cn/news/53/#c_news_list-1548139445064-1</t>
+  </si>
+  <si>
+    <t>定兴县</t>
+  </si>
+  <si>
+    <t>http://www.dingxing.gov.cn/czyslist-394-more.html</t>
+  </si>
+  <si>
+    <t>唐县</t>
+  </si>
+  <si>
+    <t>http://www.tangxian.gov.cn/czyslist-1116-more.html</t>
+  </si>
+  <si>
+    <t>高阳县</t>
+  </si>
+  <si>
+    <t>https://www.gaoyang.gov.cn/cai/</t>
   </si>
 </sst>
 </file>
@@ -179,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -194,10 +227,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,15 +531,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="55.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="55.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5">
@@ -677,10 +707,60 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21.75">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21.75">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21.75">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21.75">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21.75">
+      <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>